<commit_message>
Commit - Update 1:
- Converted data wrangling from vlookups within the excel sheet to python functions to produce additional tabs in the original excel sheet
</commit_message>
<xml_diff>
--- a/BI_Portfolio/FinProdsCompare_Proj/financial_products.xlsx
+++ b/BI_Portfolio/FinProdsCompare_Proj/financial_products.xlsx
@@ -8,6 +8,10 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Financial Products" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Products" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Average Scores" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metric Avg" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metric Scores" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,12 +440,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Product ID</t>
+          <t>ProductID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Financial Product</t>
+          <t>Product Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -501,7 +505,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Avg Score</t>
+          <t>Product Avg Score</t>
         </is>
       </c>
     </row>
@@ -982,6 +986,3300 @@
         <v>55</v>
       </c>
       <c r="N11" t="n">
+        <v>53.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Financial Product</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>60</v>
+      </c>
+      <c r="D2" t="n">
+        <v>70</v>
+      </c>
+      <c r="E2" t="n">
+        <v>85</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" t="n">
+        <v>80</v>
+      </c>
+      <c r="H2" t="n">
+        <v>60</v>
+      </c>
+      <c r="I2" t="n">
+        <v>50</v>
+      </c>
+      <c r="J2" t="n">
+        <v>70</v>
+      </c>
+      <c r="K2" t="n">
+        <v>75</v>
+      </c>
+      <c r="L2" t="n">
+        <v>80</v>
+      </c>
+      <c r="M2" t="n">
+        <v>50</v>
+      </c>
+      <c r="N2" t="n">
+        <v>66.36</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>70</v>
+      </c>
+      <c r="D3" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3" t="n">
+        <v>70</v>
+      </c>
+      <c r="F3" t="n">
+        <v>65</v>
+      </c>
+      <c r="G3" t="n">
+        <v>75</v>
+      </c>
+      <c r="H3" t="n">
+        <v>80</v>
+      </c>
+      <c r="I3" t="n">
+        <v>60</v>
+      </c>
+      <c r="J3" t="n">
+        <v>60</v>
+      </c>
+      <c r="K3" t="n">
+        <v>70</v>
+      </c>
+      <c r="L3" t="n">
+        <v>75</v>
+      </c>
+      <c r="M3" t="n">
+        <v>40</v>
+      </c>
+      <c r="N3" t="n">
+        <v>65.91</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>65</v>
+      </c>
+      <c r="D4" t="n">
+        <v>55</v>
+      </c>
+      <c r="E4" t="n">
+        <v>75</v>
+      </c>
+      <c r="F4" t="n">
+        <v>60</v>
+      </c>
+      <c r="G4" t="n">
+        <v>85</v>
+      </c>
+      <c r="H4" t="n">
+        <v>70</v>
+      </c>
+      <c r="I4" t="n">
+        <v>55</v>
+      </c>
+      <c r="J4" t="n">
+        <v>75</v>
+      </c>
+      <c r="K4" t="n">
+        <v>65</v>
+      </c>
+      <c r="L4" t="n">
+        <v>85</v>
+      </c>
+      <c r="M4" t="n">
+        <v>35</v>
+      </c>
+      <c r="N4" t="n">
+        <v>65.91</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>90</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" t="n">
+        <v>90</v>
+      </c>
+      <c r="G5" t="n">
+        <v>30</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>90</v>
+      </c>
+      <c r="K5" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" t="n">
+        <v>90</v>
+      </c>
+      <c r="M5" t="n">
+        <v>70</v>
+      </c>
+      <c r="N5" t="n">
+        <v>52.73</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+      <c r="D6" t="n">
+        <v>30</v>
+      </c>
+      <c r="E6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>70</v>
+      </c>
+      <c r="G6" t="n">
+        <v>90</v>
+      </c>
+      <c r="H6" t="n">
+        <v>15</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>95</v>
+      </c>
+      <c r="K6" t="n">
+        <v>40</v>
+      </c>
+      <c r="L6" t="n">
+        <v>95</v>
+      </c>
+      <c r="M6" t="n">
+        <v>20</v>
+      </c>
+      <c r="N6" t="n">
+        <v>50.91</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>75</v>
+      </c>
+      <c r="D7" t="n">
+        <v>40</v>
+      </c>
+      <c r="E7" t="n">
+        <v>60</v>
+      </c>
+      <c r="F7" t="n">
+        <v>55</v>
+      </c>
+      <c r="G7" t="n">
+        <v>60</v>
+      </c>
+      <c r="H7" t="n">
+        <v>75</v>
+      </c>
+      <c r="I7" t="n">
+        <v>25</v>
+      </c>
+      <c r="J7" t="n">
+        <v>80</v>
+      </c>
+      <c r="K7" t="n">
+        <v>80</v>
+      </c>
+      <c r="L7" t="n">
+        <v>70</v>
+      </c>
+      <c r="M7" t="n">
+        <v>60</v>
+      </c>
+      <c r="N7" t="n">
+        <v>61.82</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>85</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" t="n">
+        <v>75</v>
+      </c>
+      <c r="G8" t="n">
+        <v>40</v>
+      </c>
+      <c r="H8" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>85</v>
+      </c>
+      <c r="K8" t="n">
+        <v>45</v>
+      </c>
+      <c r="L8" t="n">
+        <v>80</v>
+      </c>
+      <c r="M8" t="n">
+        <v>50</v>
+      </c>
+      <c r="N8" t="n">
+        <v>49.09</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>70</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E9" t="n">
+        <v>55</v>
+      </c>
+      <c r="F9" t="n">
+        <v>45</v>
+      </c>
+      <c r="G9" t="n">
+        <v>55</v>
+      </c>
+      <c r="H9" t="n">
+        <v>55</v>
+      </c>
+      <c r="I9" t="n">
+        <v>20</v>
+      </c>
+      <c r="J9" t="n">
+        <v>70</v>
+      </c>
+      <c r="K9" t="n">
+        <v>55</v>
+      </c>
+      <c r="L9" t="n">
+        <v>75</v>
+      </c>
+      <c r="M9" t="n">
+        <v>30</v>
+      </c>
+      <c r="N9" t="n">
+        <v>52.73</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>65</v>
+      </c>
+      <c r="E10" t="n">
+        <v>80</v>
+      </c>
+      <c r="F10" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" t="n">
+        <v>70</v>
+      </c>
+      <c r="H10" t="n">
+        <v>80</v>
+      </c>
+      <c r="I10" t="n">
+        <v>35</v>
+      </c>
+      <c r="J10" t="n">
+        <v>60</v>
+      </c>
+      <c r="K10" t="n">
+        <v>85</v>
+      </c>
+      <c r="L10" t="n">
+        <v>70</v>
+      </c>
+      <c r="M10" t="n">
+        <v>65</v>
+      </c>
+      <c r="N10" t="n">
+        <v>65.45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" t="n">
+        <v>75</v>
+      </c>
+      <c r="E11" t="n">
+        <v>65</v>
+      </c>
+      <c r="F11" t="n">
+        <v>40</v>
+      </c>
+      <c r="G11" t="n">
+        <v>75</v>
+      </c>
+      <c r="H11" t="n">
+        <v>45</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" t="n">
+        <v>50</v>
+      </c>
+      <c r="K11" t="n">
+        <v>65</v>
+      </c>
+      <c r="L11" t="n">
+        <v>60</v>
+      </c>
+      <c r="M11" t="n">
+        <v>55</v>
+      </c>
+      <c r="N11" t="n">
+        <v>53.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Average Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>47.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Average Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>47.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ProductID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Stability</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Potential Earnings</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Tax Friendly</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Diversification</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Management Fees</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Minimum Investment</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Historical Performance</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Ease of Access</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Inflation Hedge</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Individual Securities</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>66.36</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Mutual Funds</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>65.91</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>ETFs</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>65.91</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>P4</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Government Bonds</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>52.73</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>P5</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>High Yield Savings Account</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>50.91</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>P6</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Real Estate Investment Trusts (REITs)</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>61.82</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>P7</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Certificates of Deposit (CDs)</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>49.09</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>P8</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Corporate Bonds</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>52.73</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Dividend Stocks</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>65.45</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>P10</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Peer-to-Peer Lending</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Product Avg Score</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
         <v>53.64</v>
       </c>
     </row>

</xml_diff>